<commit_message>
Add LTC6811 libraries to BMS
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aman/Documents/Berkeley/Clubs/Formula Electric/CAN Bus/Header Generation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aman/Documents/Berkeley/Clubs/FEB/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458C139A-2E56-DD4A-BD68-1DF4D810B45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB8A833-7A79-CA4D-BEA0-90FE89FD4675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30060" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t xml:space="preserve">Torque </t>
+  </si>
+  <si>
+    <t>Set Address</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Voltage 1</t>
+  </si>
+  <si>
+    <t>Voltage 2</t>
+  </si>
+  <si>
+    <t>Voltage 3</t>
+  </si>
+  <si>
+    <t>uint32_t</t>
+  </si>
+  <si>
+    <t>IVT_CURRENT</t>
   </si>
 </sst>
 </file>
@@ -648,7 +669,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -672,19 +693,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1042,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F11" sqref="A1:F11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1054,7 +1081,7 @@
     <col min="6" max="6" width="16.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1073,40 +1100,45 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>11</v>
       </c>
       <c r="B2" s="5">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C3" s="11"/>
-      <c r="D3" s="10"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="9"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="11" t="s">
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1115,18 +1147,20 @@
       <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1139,12 +1173,13 @@
       <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="12" t="s">
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1153,38 +1188,42 @@
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="10"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C9" s="12"/>
-      <c r="D9" s="11"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="10"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="13" t="s">
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1195,6 +1234,47 @@
       <c r="F11" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Block IDs in CAN Library
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aman/Documents/Berkeley/Clubs/FEB/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB8A833-7A79-CA4D-BEA0-90FE89FD4675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665165D8-090D-9945-AC6E-FDCEA6118731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30060" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="identifiers" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -107,25 +108,49 @@
     <t xml:space="preserve">Torque </t>
   </si>
   <si>
-    <t>Set Address</t>
-  </si>
-  <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>Voltage 1</t>
-  </si>
-  <si>
-    <t>Voltage 2</t>
-  </si>
-  <si>
-    <t>Voltage 3</t>
-  </si>
-  <si>
-    <t>uint32_t</t>
-  </si>
-  <si>
-    <t>IVT_CURRENT</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Receive (T/F)</t>
+  </si>
+  <si>
+    <t>IVT_Current</t>
+  </si>
+  <si>
+    <t>IVT_Voltage1</t>
+  </si>
+  <si>
+    <t>IVT_Voltage2</t>
+  </si>
+  <si>
+    <t>IVT_Voltage3</t>
+  </si>
+  <si>
+    <t>0x521</t>
+  </si>
+  <si>
+    <t>0x522</t>
+  </si>
+  <si>
+    <t>0x523</t>
+  </si>
+  <si>
+    <t>0x524</t>
+  </si>
+  <si>
+    <t>uint8_t[6]</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Rx Any (T/F)</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -669,7 +694,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -693,6 +718,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -705,13 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1071,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1101,7 +1123,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1111,21 +1133,23 @@
       <c r="B2" s="5">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="9"/>
-      <c r="D3" s="12"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
@@ -1135,10 +1159,10 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1147,11 +1171,13 @@
       <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1173,13 +1199,15 @@
       <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1188,11 +1216,13 @@
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="10"/>
-      <c r="D8" s="9"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1202,8 +1232,8 @@
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1213,8 +1243,8 @@
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="10"/>
-      <c r="D10" s="9"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1234,46 +1264,30 @@
       <c r="F11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E13" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E15" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="7"/>
     </row>
   </sheetData>
@@ -1287,4 +1301,93 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DC653-96F5-104F-BB32-C847D8C928AF}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Temp LUT to BMS
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aman/Documents/Berkeley/Clubs/FEB/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665165D8-090D-9945-AC6E-FDCEA6118731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17496FB6-C90B-1C4D-8D18-48344DFF7693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30060" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -623,32 +626,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -718,24 +695,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1091,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H2" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,7 +1078,7 @@
     <col min="6" max="6" width="16.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1125,18 +1100,21 @@
       <c r="G1" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>11</v>
       </c>
       <c r="B2" s="5">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="7" t="s">
         <v>20</v>
       </c>
@@ -1146,10 +1124,11 @@
       <c r="G2" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="10"/>
-      <c r="D3" s="13"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
@@ -1157,12 +1136,13 @@
         <v>13</v>
       </c>
       <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C4" s="10" t="s">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1174,10 +1154,11 @@
       <c r="G4" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1185,8 +1166,9 @@
         <v>9</v>
       </c>
       <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1202,12 +1184,13 @@
       <c r="G6" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="11" t="s">
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1219,10 +1202,11 @@
       <c r="G7" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="11"/>
-      <c r="D8" s="10"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C8" s="10"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1230,10 +1214,11 @@
         <v>9</v>
       </c>
       <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C9" s="10"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1241,10 +1226,11 @@
         <v>9</v>
       </c>
       <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="11"/>
-      <c r="D10" s="10"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1252,8 +1238,9 @@
         <v>9</v>
       </c>
       <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1264,31 +1251,40 @@
       <c r="F11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="14"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1308,7 +1304,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,16 +1314,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BMS balance cells while charging
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aman/Documents/Berkeley/Clubs/FEB/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17496FB6-C90B-1C4D-8D18-48344DFF7693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FD6884-8365-DB49-A068-559E1878CA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30060" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -117,24 +117,9 @@
     <t>Receive (T/F)</t>
   </si>
   <si>
-    <t>IVT_Current</t>
-  </si>
-  <si>
-    <t>IVT_Voltage1</t>
-  </si>
-  <si>
-    <t>IVT_Voltage2</t>
-  </si>
-  <si>
-    <t>IVT_Voltage3</t>
-  </si>
-  <si>
     <t>0x521</t>
   </si>
   <si>
-    <t>0x522</t>
-  </si>
-  <si>
     <t>0x523</t>
   </si>
   <si>
@@ -154,6 +139,66 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Command</t>
+  </si>
+  <si>
+    <t>0x411</t>
+  </si>
+  <si>
+    <t>uint8_t[8]</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Debug</t>
+  </si>
+  <si>
+    <t>0x510</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Response</t>
+  </si>
+  <si>
+    <t>0x511</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Result_I</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Result_U1</t>
+  </si>
+  <si>
+    <t>0X522</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Result_U2</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Result_U3</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Result_T</t>
+  </si>
+  <si>
+    <t>0x525</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Result_W</t>
+  </si>
+  <si>
+    <t>0x526</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Result_As</t>
+  </si>
+  <si>
+    <t>0x527</t>
+  </si>
+  <si>
+    <t>IVT_Msg_Result_Wh</t>
+  </si>
+  <si>
+    <t>0x528</t>
   </si>
 </sst>
 </file>
@@ -671,7 +716,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -695,22 +740,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,13 +1112,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H11"/>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="16.83203125" style="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" style="8"/>
   </cols>
   <sheetData>
@@ -1098,10 +1143,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1111,61 +1156,61 @@
       <c r="B2" s="5">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>38</v>
+      <c r="G2" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="7" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>36</v>
+      <c r="G4" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1175,69 +1220,69 @@
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="13" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>38</v>
+      <c r="G6" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>38</v>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="10"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="3" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="3" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="10"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="13" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1247,44 +1292,25 @@
       <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="C12" s="8"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="14"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="14"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="14"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="E15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1301,87 +1327,209 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DC653-96F5-104F-BB32-C847D8C928AF}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="183" workbookViewId="0">
+      <selection activeCell="D12" sqref="A2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update BMS IVT code
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aman/Documents/Berkeley/Clubs/FEB/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FD6884-8365-DB49-A068-559E1878CA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB3E627-C371-5F4D-BD83-44E4E9C311C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -716,7 +716,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -744,16 +744,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1112,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="D16" activeCellId="1" sqref="E5 D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1156,11 +1153,11 @@
       <c r="B2" s="5">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1172,9 +1169,9 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="13" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="10" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1184,13 +1181,13 @@
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -1202,9 +1199,9 @@
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="13" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -1220,7 +1217,7 @@
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1232,13 +1229,13 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1250,9 +1247,9 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="11"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -1262,9 +1259,9 @@
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1274,9 +1271,9 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="11"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="13" t="s">
+      <c r="C10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -1292,7 +1289,7 @@
       <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1329,7 +1326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DC653-96F5-104F-BB32-C847D8C928AF}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" workbookViewId="0">
+    <sheetView zoomScale="183" workbookViewId="0">
       <selection activeCell="D12" sqref="A2:D12"/>
     </sheetView>
   </sheetViews>
@@ -1508,28 +1505,28 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated node excel and header file
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aman/Documents/Berkeley/Clubs/FEB/FEB_Firmware_2023/CAN_Library/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imasmm/Academic/feb/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB3E627-C371-5F4D-BD83-44E4E9C311C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B170745-85C6-7744-BD6B-97B6E2315084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>BMS</t>
   </si>
   <si>
-    <t>SM</t>
-  </si>
-  <si>
     <t>Temperature</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>APPS_Emergency</t>
   </si>
   <si>
-    <t>SM_Emergency</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -199,6 +193,12 @@
   </si>
   <si>
     <t>0x528</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>SW_Emergency</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="D16" activeCellId="1" sqref="E5 D16"/>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,10 +1140,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1154,17 +1154,17 @@
         <v>7</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="7"/>
     </row>
@@ -1172,10 +1172,10 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="10" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="7"/>
@@ -1185,16 +1185,16 @@
         <v>6</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -1202,47 +1202,47 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H7" s="7"/>
     </row>
@@ -1250,10 +1250,10 @@
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
       <c r="E8" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="7"/>
@@ -1262,10 +1262,10 @@
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
       <c r="E9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="7"/>
@@ -1274,24 +1274,24 @@
       <c r="C10" s="12"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="7"/>
@@ -1324,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DC653-96F5-104F-BB32-C847D8C928AF}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScale="183" workbookViewId="0">
-      <selection activeCell="D12" sqref="A2:D12"/>
+    <sheetView tabSelected="1" zoomScale="183" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1338,195 +1338,171 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding LVPDB node to excel
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imasmm/Academic/feb/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B170745-85C6-7744-BD6B-97B6E2315084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ECEC16-F302-3341-BE1F-F912704EC763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Brake Pedal</t>
   </si>
   <si>
-    <t>BMS APPS</t>
-  </si>
-  <si>
     <t>Command 1</t>
   </si>
   <si>
@@ -199,6 +196,12 @@
   </si>
   <si>
     <t>SW_Emergency</t>
+  </si>
+  <si>
+    <t>IVPDB</t>
+  </si>
+  <si>
+    <t>BMS SW</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,10 +1143,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1154,17 +1157,17 @@
         <v>7</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="7"/>
     </row>
@@ -1172,7 +1175,7 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>12</v>
@@ -1185,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>7</v>
@@ -1194,7 +1197,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -1212,19 +1215,17 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -1233,7 +1234,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>13</v>
@@ -1242,7 +1243,7 @@
         <v>8</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H7" s="7"/>
     </row>
@@ -1274,7 +1275,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>8</v>
@@ -1287,18 +1288,32 @@
         <v>11</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="C12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E13" s="8"/>
@@ -1326,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DC653-96F5-104F-BB32-C847D8C928AF}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" workbookViewId="0">
+    <sheetView zoomScale="183" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:D16"/>
     </sheetView>
   </sheetViews>
@@ -1338,170 +1353,170 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving, hardcoding inverter ids
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aman/Documents/Berkeley/Clubs/FEB/FEB_Firmware_2023/CAN_Library/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imasmm/Academic/feb/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB3E627-C371-5F4D-BD83-44E4E9C311C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8B29A7-1EC3-9942-B884-9B3C7624D83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -57,9 +57,6 @@
     <t>BMS</t>
   </si>
   <si>
-    <t>SM</t>
-  </si>
-  <si>
     <t>Temperature</t>
   </si>
   <si>
@@ -87,21 +84,12 @@
     <t>Brake Pedal</t>
   </si>
   <si>
-    <t>BMS APPS</t>
-  </si>
-  <si>
-    <t>Command 1</t>
-  </si>
-  <si>
     <t>Emergency</t>
   </si>
   <si>
     <t>APPS_Emergency</t>
   </si>
   <si>
-    <t>SM_Emergency</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -199,6 +187,30 @@
   </si>
   <si>
     <t>0x528</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>SW_Emergency</t>
+  </si>
+  <si>
+    <t>IVPDB</t>
+  </si>
+  <si>
+    <t>BMS SW</t>
+  </si>
+  <si>
+    <t>Ready_to_drive</t>
+  </si>
+  <si>
+    <t>Coolant_pump</t>
+  </si>
+  <si>
+    <t>Acumulator_fans</t>
+  </si>
+  <si>
+    <t>Extra</t>
   </si>
 </sst>
 </file>
@@ -528,7 +540,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -671,6 +683,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -716,7 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -751,6 +800,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1107,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="D16" activeCellId="1" sqref="E5 D16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,10 +1198,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1154,17 +1212,17 @@
         <v>7</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H2" s="7"/>
     </row>
@@ -1172,10 +1230,10 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="10" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="7"/>
@@ -1185,16 +1243,16 @@
         <v>6</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -1202,121 +1260,171 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="C6" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="13"/>
       <c r="E6" s="10" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>7</v>
-      </c>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="10" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>33</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="10" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="12"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="10" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
+    <row r="10" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="E10" s="10" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F11" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E13" s="8"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E14" s="8"/>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E15" s="8"/>
+      <c r="C15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
     <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1324,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DC653-96F5-104F-BB32-C847D8C928AF}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="183" workbookViewId="0">
-      <selection activeCell="D12" sqref="A2:D12"/>
+      <selection activeCell="A13" sqref="A13:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1338,195 +1446,171 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working buttons for peripheral devices
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imasmm/Academic/feb/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCD13DC-5FAC-3B43-84FB-FB73D48E0288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4100BCC5-66CF-C549-8AEA-10E81CB70246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Brake Pedal</t>
   </si>
   <si>
-    <t>Command 1</t>
-  </si>
-  <si>
     <t>Emergency</t>
   </si>
   <si>
@@ -201,10 +198,19 @@
     <t>BMS SW</t>
   </si>
   <si>
+    <t>Ready_to_drive</t>
+  </si>
+  <si>
+    <t>Coolant_pump</t>
+  </si>
+  <si>
+    <t>Acumulator_fans</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
     <t>LVPDB</t>
-  </si>
-  <si>
-    <t>SW APPS</t>
   </si>
 </sst>
 </file>
@@ -534,7 +540,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -677,6 +683,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -722,7 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -757,6 +800,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1113,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1146,10 +1198,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1160,17 +1212,17 @@
         <v>7</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="7"/>
     </row>
@@ -1178,7 +1230,7 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>12</v>
@@ -1191,7 +1243,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>7</v>
@@ -1200,7 +1252,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -1217,124 +1269,162 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="6"/>
+      <c r="C6" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="13"/>
       <c r="E6" s="10" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>54</v>
-      </c>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="10" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="10" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="12"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="10" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
+    <row r="10" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="E10" s="10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="12"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="12"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E14" s="8"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E15" s="8"/>
+      <c r="C15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
     <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1356,170 +1446,170 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added RMS IDs, modified string format
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imasmm/Academic/feb/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8B29A7-1EC3-9942-B884-9B3C7624D83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740BED82-BF48-DF4B-8DE2-E957C48216EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="110">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -69,9 +69,6 @@
     <t>APPS</t>
   </si>
   <si>
-    <t>RMS</t>
-  </si>
-  <si>
     <t>uint8_t</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>SW_Emergency</t>
   </si>
   <si>
-    <t>IVPDB</t>
-  </si>
-  <si>
     <t>BMS SW</t>
   </si>
   <si>
@@ -211,13 +205,172 @@
   </si>
   <si>
     <t>Extra</t>
+  </si>
+  <si>
+    <t>LVPDB</t>
+  </si>
+  <si>
+    <t>RMS_Temperature1</t>
+  </si>
+  <si>
+    <t>RMS_Temperature2</t>
+  </si>
+  <si>
+    <t>RMS_Temperature3</t>
+  </si>
+  <si>
+    <t>0x0A0</t>
+  </si>
+  <si>
+    <t>0x0A1</t>
+  </si>
+  <si>
+    <t>0x0A2</t>
+  </si>
+  <si>
+    <t>0x0A3</t>
+  </si>
+  <si>
+    <t>0x0A4</t>
+  </si>
+  <si>
+    <t>0x0A5</t>
+  </si>
+  <si>
+    <t>0x0A6</t>
+  </si>
+  <si>
+    <t>0x0A7</t>
+  </si>
+  <si>
+    <t>0x0A8</t>
+  </si>
+  <si>
+    <t>0x0A9</t>
+  </si>
+  <si>
+    <t>0x0AA</t>
+  </si>
+  <si>
+    <t>0x0AB</t>
+  </si>
+  <si>
+    <t>0x0AC</t>
+  </si>
+  <si>
+    <t>0x0AD</t>
+  </si>
+  <si>
+    <t>0x0AE</t>
+  </si>
+  <si>
+    <t>0x0AF</t>
+  </si>
+  <si>
+    <t>0x0B0</t>
+  </si>
+  <si>
+    <t>RMS_Analog_Input_Voltages</t>
+  </si>
+  <si>
+    <t>RMS_Digital_Input_Status</t>
+  </si>
+  <si>
+    <t>RMS_Motor_Position_Info</t>
+  </si>
+  <si>
+    <t>RMS_Current</t>
+  </si>
+  <si>
+    <t>RMS_Voltage</t>
+  </si>
+  <si>
+    <t>RMS_Flux</t>
+  </si>
+  <si>
+    <t>RMS_Internal_Votages</t>
+  </si>
+  <si>
+    <t>RMS_Internal_States</t>
+  </si>
+  <si>
+    <t>RMS_Fault_Coes</t>
+  </si>
+  <si>
+    <t>RMS_Torque_Timer</t>
+  </si>
+  <si>
+    <t>RMS_Modulation_Index_Flux_Weakening_Output</t>
+  </si>
+  <si>
+    <t>RMS_Firmware_Info</t>
+  </si>
+  <si>
+    <t>RMS_Diagnostic_Data</t>
+  </si>
+  <si>
+    <t>RMS_High_Speed_Msg</t>
+  </si>
+  <si>
+    <t>RMS_Cmd_Msg</t>
+  </si>
+  <si>
+    <t>0x0C0</t>
+  </si>
+  <si>
+    <t>RMS_Param_Cmd</t>
+  </si>
+  <si>
+    <t>RMS_Param_Response</t>
+  </si>
+  <si>
+    <t>0x0C1</t>
+  </si>
+  <si>
+    <t>0x0C2</t>
+  </si>
+  <si>
+    <t>RMS_OBD2_Query</t>
+  </si>
+  <si>
+    <t>RMS_OBD2_Respond</t>
+  </si>
+  <si>
+    <t>0x7DF</t>
+  </si>
+  <si>
+    <t>0x7E7</t>
+  </si>
+  <si>
+    <t>RMS_Orion_BMS</t>
+  </si>
+  <si>
+    <t>0x202</t>
+  </si>
+  <si>
+    <t>RMS_Debouce_Counter_Max_EEPROM</t>
+  </si>
+  <si>
+    <t>0x0EE</t>
+  </si>
+  <si>
+    <t>RMS_Debounce_Up_Count_EEPROM</t>
+  </si>
+  <si>
+    <t>0x0EF</t>
+  </si>
+  <si>
+    <t>RMS_Debounce_Down_Count_EEPROM</t>
+  </si>
+  <si>
+    <t>0x0F0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -351,6 +504,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -765,7 +930,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -804,11 +969,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1165,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1198,10 +1371,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1212,17 +1385,17 @@
         <v>7</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="7"/>
     </row>
@@ -1230,10 +1403,10 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="7"/>
@@ -1243,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>7</v>
@@ -1252,7 +1425,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -1270,52 +1443,52 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="7"/>
@@ -1325,16 +1498,16 @@
         <v>10</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="7"/>
     </row>
@@ -1342,7 +1515,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="11"/>
       <c r="E11" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>8</v>
@@ -1354,7 +1527,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>8</v>
@@ -1366,7 +1539,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="11"/>
       <c r="E13" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>8</v>
@@ -1376,44 +1549,28 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15" s="7"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1432,187 +1589,552 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DC653-96F5-104F-BB32-C847D8C928AF}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView zoomScale="183" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="183" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed not receiving APPS
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imasmm/Academic/feb/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740BED82-BF48-DF4B-8DE2-E957C48216EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BB4301-0E7A-734D-BC0D-9C27D32F0F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="111">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>0x0F0</t>
+  </si>
+  <si>
+    <t>SW APPS</t>
   </si>
 </sst>
 </file>
@@ -930,7 +933,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -960,6 +963,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -974,14 +982,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1340,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1384,10 +1384,10 @@
       <c r="B2" s="5">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="10" t="s">
         <v>16</v>
       </c>
@@ -1400,8 +1400,8 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="10" t="s">
         <v>51</v>
       </c>
@@ -1412,10 +1412,10 @@
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="14" t="s">
         <v>50</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -1430,8 +1430,8 @@
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1442,10 +1442,10 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="13"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="10" t="s">
         <v>53</v>
       </c>
@@ -1458,8 +1458,8 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="10" t="s">
         <v>54</v>
       </c>
@@ -1470,8 +1470,8 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="10" t="s">
         <v>55</v>
       </c>
@@ -1482,8 +1482,8 @@
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="10" t="s">
         <v>56</v>
       </c>
@@ -1494,10 +1494,10 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="14" t="s">
         <v>52</v>
       </c>
       <c r="E10" s="10" t="s">
@@ -1512,8 +1512,8 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="10" t="s">
         <v>13</v>
       </c>
@@ -1524,8 +1524,8 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="12"/>
-      <c r="D12" s="11"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="10" t="s">
         <v>14</v>
       </c>
@@ -1536,8 +1536,8 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="12"/>
-      <c r="D13" s="11"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>57</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="3" t="s">
@@ -1591,7 +1591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DC653-96F5-104F-BB32-C847D8C928AF}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="183" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="183" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -1770,30 +1770,30 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="17" t="s">
+      <c r="C13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="17" t="s">
+      <c r="C14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1801,13 +1801,13 @@
       <c r="A15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="17" t="s">
+      <c r="C15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1815,13 +1815,13 @@
       <c r="A16" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="17" t="s">
+      <c r="C16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1829,27 +1829,27 @@
       <c r="A17" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="17" t="s">
+      <c r="C17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="17" t="s">
+      <c r="C18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1857,13 +1857,13 @@
       <c r="A19" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="C19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1871,13 +1871,13 @@
       <c r="A20" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="17" t="s">
+      <c r="C20" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1885,13 +1885,13 @@
       <c r="A21" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="17" t="s">
+      <c r="C21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1899,13 +1899,13 @@
       <c r="A22" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="17" t="s">
+      <c r="C22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1913,13 +1913,13 @@
       <c r="A23" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="17" t="s">
+      <c r="C23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1927,13 +1927,13 @@
       <c r="A24" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1941,13 +1941,13 @@
       <c r="A25" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="17" t="s">
+      <c r="C25" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1955,13 +1955,13 @@
       <c r="A26" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="17" t="s">
+      <c r="C26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1969,13 +1969,13 @@
       <c r="A27" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="17" t="s">
+      <c r="C27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1983,13 +1983,13 @@
       <c r="A28" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1997,13 +1997,13 @@
       <c r="A29" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="17" t="s">
+      <c r="C29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2011,13 +2011,13 @@
       <c r="A30" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="17" t="s">
+      <c r="C30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2025,13 +2025,13 @@
       <c r="A31" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="19" t="s">
+      <c r="C31" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2039,13 +2039,13 @@
       <c r="A32" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="19" t="s">
+      <c r="C32" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2053,13 +2053,13 @@
       <c r="A33" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="19" t="s">
+      <c r="C33" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2067,13 +2067,13 @@
       <c r="A34" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="19" t="s">
+      <c r="C34" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2081,13 +2081,13 @@
       <c r="A35" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="19" t="s">
+      <c r="C35" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2095,13 +2095,13 @@
       <c r="A36" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="19" t="s">
+      <c r="C36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2109,13 +2109,13 @@
       <c r="A37" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="19" t="s">
+      <c r="C37" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2123,13 +2123,13 @@
       <c r="A38" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D38" s="19" t="s">
+      <c r="C38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed node id list
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imasmm/Academic/feb/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8B29A7-1EC3-9942-B884-9B3C7624D83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9742C403-C7C4-F845-A1C2-AE05285F0D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="111">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -69,9 +69,6 @@
     <t>APPS</t>
   </si>
   <si>
-    <t>RMS</t>
-  </si>
-  <si>
     <t>uint8_t</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>SW_Emergency</t>
   </si>
   <si>
-    <t>IVPDB</t>
-  </si>
-  <si>
     <t>BMS SW</t>
   </si>
   <si>
@@ -211,13 +205,175 @@
   </si>
   <si>
     <t>Extra</t>
+  </si>
+  <si>
+    <t>LVPDB</t>
+  </si>
+  <si>
+    <t>RMS_Temperature1</t>
+  </si>
+  <si>
+    <t>RMS_Temperature2</t>
+  </si>
+  <si>
+    <t>RMS_Temperature3</t>
+  </si>
+  <si>
+    <t>0x0A0</t>
+  </si>
+  <si>
+    <t>0x0A1</t>
+  </si>
+  <si>
+    <t>0x0A2</t>
+  </si>
+  <si>
+    <t>0x0A3</t>
+  </si>
+  <si>
+    <t>0x0A4</t>
+  </si>
+  <si>
+    <t>0x0A5</t>
+  </si>
+  <si>
+    <t>0x0A6</t>
+  </si>
+  <si>
+    <t>0x0A7</t>
+  </si>
+  <si>
+    <t>0x0A8</t>
+  </si>
+  <si>
+    <t>0x0A9</t>
+  </si>
+  <si>
+    <t>0x0AA</t>
+  </si>
+  <si>
+    <t>0x0AB</t>
+  </si>
+  <si>
+    <t>0x0AC</t>
+  </si>
+  <si>
+    <t>0x0AD</t>
+  </si>
+  <si>
+    <t>0x0AE</t>
+  </si>
+  <si>
+    <t>0x0AF</t>
+  </si>
+  <si>
+    <t>0x0B0</t>
+  </si>
+  <si>
+    <t>RMS_Analog_Input_Voltages</t>
+  </si>
+  <si>
+    <t>RMS_Digital_Input_Status</t>
+  </si>
+  <si>
+    <t>RMS_Motor_Position_Info</t>
+  </si>
+  <si>
+    <t>RMS_Current</t>
+  </si>
+  <si>
+    <t>RMS_Voltage</t>
+  </si>
+  <si>
+    <t>RMS_Flux</t>
+  </si>
+  <si>
+    <t>RMS_Internal_Votages</t>
+  </si>
+  <si>
+    <t>RMS_Internal_States</t>
+  </si>
+  <si>
+    <t>RMS_Fault_Coes</t>
+  </si>
+  <si>
+    <t>RMS_Torque_Timer</t>
+  </si>
+  <si>
+    <t>RMS_Modulation_Index_Flux_Weakening_Output</t>
+  </si>
+  <si>
+    <t>RMS_Firmware_Info</t>
+  </si>
+  <si>
+    <t>RMS_Diagnostic_Data</t>
+  </si>
+  <si>
+    <t>RMS_High_Speed_Msg</t>
+  </si>
+  <si>
+    <t>RMS_Cmd_Msg</t>
+  </si>
+  <si>
+    <t>0x0C0</t>
+  </si>
+  <si>
+    <t>RMS_Param_Cmd</t>
+  </si>
+  <si>
+    <t>RMS_Param_Response</t>
+  </si>
+  <si>
+    <t>0x0C1</t>
+  </si>
+  <si>
+    <t>0x0C2</t>
+  </si>
+  <si>
+    <t>RMS_OBD2_Query</t>
+  </si>
+  <si>
+    <t>RMS_OBD2_Respond</t>
+  </si>
+  <si>
+    <t>0x7DF</t>
+  </si>
+  <si>
+    <t>0x7E7</t>
+  </si>
+  <si>
+    <t>RMS_Orion_BMS</t>
+  </si>
+  <si>
+    <t>0x202</t>
+  </si>
+  <si>
+    <t>RMS_Debouce_Counter_Max_EEPROM</t>
+  </si>
+  <si>
+    <t>0x0EE</t>
+  </si>
+  <si>
+    <t>RMS_Debounce_Up_Count_EEPROM</t>
+  </si>
+  <si>
+    <t>0x0EF</t>
+  </si>
+  <si>
+    <t>RMS_Debounce_Down_Count_EEPROM</t>
+  </si>
+  <si>
+    <t>0x0F0</t>
+  </si>
+  <si>
+    <t>SW APPS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -351,6 +507,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -765,7 +933,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -795,6 +963,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -804,10 +977,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1165,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1198,10 +1371,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1211,39 +1384,39 @@
       <c r="B2" s="5">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>51</v>
+      <c r="D4" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>7</v>
@@ -1252,13 +1425,13 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1269,80 +1442,80 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="13"/>
+      <c r="C6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="16"/>
       <c r="E6" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>54</v>
+      <c r="D10" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>8</v>
@@ -1351,10 +1524,10 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="12"/>
-      <c r="D12" s="11"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>8</v>
@@ -1363,10 +1536,10 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="12"/>
-      <c r="D13" s="11"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>8</v>
@@ -1376,44 +1549,28 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15" s="7"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1432,187 +1589,552 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DC653-96F5-104F-BB32-C847D8C928AF}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView zoomScale="183" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:D16"/>
+    <sheetView topLeftCell="A11" zoomScale="183" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code flashed before leaving for comp
</commit_message>
<xml_diff>
--- a/CAN_Library/data.xlsx
+++ b/CAN_Library/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imasmm/Academic/feb/FEB_Firmware_2023/CAN_Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9742C403-C7C4-F845-A1C2-AE05285F0D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556D5523-80D9-024C-89B9-B8D980FE39C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="111">
   <si>
     <t>CAN ID Length</t>
   </si>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D6" sqref="D6:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1445,7 +1445,9 @@
       <c r="C6" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" s="10" t="s">
         <v>53</v>
       </c>

</xml_diff>